<commit_message>
Projeto Web TDD finalizado
</commit_message>
<xml_diff>
--- a/src/test/resources/Excel/Massa.xlsx
+++ b/src/test/resources/Excel/Massa.xlsx
@@ -3,35 +3,26 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\victor.albano\Documents\Victor\Massa\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{630DCBC2-3994-47AF-95C6-73ECCE3BBA2E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{0C8830E7-FBA6-4119-9870-47E78828AD86}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{42C517F9-3C2F-4E44-A03E-BA06A54FC42C}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="20640" windowHeight="15660" activeTab="1" xr2:uid="{42C517F9-3C2F-4E44-A03E-BA06A54FC42C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Login" sheetId="1" r:id="rId1"/>
+    <sheet name="Cadastro" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:I18"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
   <si>
     <t>Usuario</t>
   </si>
@@ -49,13 +40,91 @@
   </si>
   <si>
     <t>Abc3</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>PhoneNumber</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Adress</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>PostalCode</t>
+  </si>
+  <si>
+    <t>Victor</t>
+  </si>
+  <si>
+    <t>Albano</t>
+  </si>
+  <si>
+    <t>Brazil</t>
+  </si>
+  <si>
+    <t>Santo Andre</t>
+  </si>
+  <si>
+    <t>Rua Natal</t>
+  </si>
+  <si>
+    <t>SP</t>
+  </si>
+  <si>
+    <t>rodrigo</t>
+  </si>
+  <si>
+    <t>rodrigo1@gmail.com</t>
+  </si>
+  <si>
+    <t>Rodrigo</t>
+  </si>
+  <si>
+    <t>Morais</t>
+  </si>
+  <si>
+    <t>11953459764</t>
+  </si>
+  <si>
+    <t>11990909898</t>
+  </si>
+  <si>
+    <t>09030600</t>
+  </si>
+  <si>
+    <t>09030601</t>
+  </si>
+  <si>
+    <t>VictorAlbanoV17</t>
+  </si>
+  <si>
+    <t>victoralbanoV17@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -66,6 +135,22 @@
     <font>
       <b/>
       <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -110,10 +195,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -124,8 +210,19 @@
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -438,26 +535,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82DFF3C8-B17A-4903-B3D2-C0FC0EFDC6B7}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>2</v>
       </c>
+      <c r="H1" s="7"/>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -465,7 +570,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -473,8 +578,145 @@
         <v>5</v>
       </c>
     </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{502FE14B-E947-42A8-81A3-4901D77307AB}">
+  <dimension ref="A1:K3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{8496FEEB-E748-4C8D-8E35-BC08CB25A0A3}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{EB71E9ED-9D42-4256-B380-9583AD4D17EB}"/>
+  </hyperlinks>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Refatorando PageObjects e organizando testes
</commit_message>
<xml_diff>
--- a/src/test/resources/Excel/Massa.xlsx
+++ b/src/test/resources/Excel/Massa.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{0C8830E7-FBA6-4119-9870-47E78828AD86}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{271B0F41-64FB-4FB9-AF41-E09056A71837}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="20640" windowHeight="15660" activeTab="1" xr2:uid="{42C517F9-3C2F-4E44-A03E-BA06A54FC42C}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="20760" windowHeight="15660" xr2:uid="{42C517F9-3C2F-4E44-A03E-BA06A54FC42C}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -72,52 +72,52 @@
     <t>PostalCode</t>
   </si>
   <si>
+    <t>Albano</t>
+  </si>
+  <si>
+    <t>Brazil</t>
+  </si>
+  <si>
+    <t>Santo Andre</t>
+  </si>
+  <si>
+    <t>Rua Natal</t>
+  </si>
+  <si>
+    <t>SP</t>
+  </si>
+  <si>
+    <t>rodrigo</t>
+  </si>
+  <si>
+    <t>rodrigo1@gmail.com</t>
+  </si>
+  <si>
+    <t>Rodrigo</t>
+  </si>
+  <si>
+    <t>Morais</t>
+  </si>
+  <si>
+    <t>11990909898</t>
+  </si>
+  <si>
+    <t>09030600</t>
+  </si>
+  <si>
+    <t>09030601</t>
+  </si>
+  <si>
+    <t>VictorAlbanoV17</t>
+  </si>
+  <si>
+    <t>victoralbanoV17@gmail.com</t>
+  </si>
+  <si>
     <t>Victor</t>
   </si>
   <si>
-    <t>Albano</t>
-  </si>
-  <si>
-    <t>Brazil</t>
-  </si>
-  <si>
-    <t>Santo Andre</t>
-  </si>
-  <si>
-    <t>Rua Natal</t>
-  </si>
-  <si>
-    <t>SP</t>
-  </si>
-  <si>
-    <t>rodrigo</t>
-  </si>
-  <si>
-    <t>rodrigo1@gmail.com</t>
-  </si>
-  <si>
-    <t>Rodrigo</t>
-  </si>
-  <si>
-    <t>Morais</t>
-  </si>
-  <si>
     <t>11953459764</t>
-  </si>
-  <si>
-    <t>11990909898</t>
-  </si>
-  <si>
-    <t>09030600</t>
-  </si>
-  <si>
-    <t>09030601</t>
-  </si>
-  <si>
-    <t>VictorAlbanoV17</t>
-  </si>
-  <si>
-    <t>victoralbanoV17@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -537,8 +537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82DFF3C8-B17A-4903-B3D2-C0FC0EFDC6B7}">
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:K7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -591,8 +591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{502FE14B-E947-42A8-81A3-4901D77307AB}">
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -644,72 +644,72 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="H2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" s="5" t="s">
         <v>26</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="E3" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="F3" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="G3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" s="5" t="s">
         <v>27</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="K3" s="5" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Pequena refatoracao. Projeto finalizado
</commit_message>
<xml_diff>
--- a/src/test/resources/Excel/Massa.xlsx
+++ b/src/test/resources/Excel/Massa.xlsx
@@ -3,16 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{271B0F41-64FB-4FB9-AF41-E09056A71837}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{B8CA4F6E-43A5-4EB8-8C88-4B4D7338AC55}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="20760" windowHeight="15660" xr2:uid="{42C517F9-3C2F-4E44-A03E-BA06A54FC42C}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="20790" windowHeight="11820" activeTab="1" xr2:uid="{42C517F9-3C2F-4E44-A03E-BA06A54FC42C}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
     <sheet name="Cadastro" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:I18"/>
+  <oleSize ref="A1:J9"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -537,7 +537,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82DFF3C8-B17A-4903-B3D2-C0FC0EFDC6B7}">
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -591,7 +591,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{502FE14B-E947-42A8-81A3-4901D77307AB}">
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Alterando massa de dados. Códigos permanecem iguais. Projeto finalizado
</commit_message>
<xml_diff>
--- a/src/test/resources/Excel/Massa.xlsx
+++ b/src/test/resources/Excel/Massa.xlsx
@@ -3,16 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{B8CA4F6E-43A5-4EB8-8C88-4B4D7338AC55}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{B57FB169-1233-42D9-B526-011535BC7F3A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="20790" windowHeight="11820" activeTab="1" xr2:uid="{42C517F9-3C2F-4E44-A03E-BA06A54FC42C}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="20850" windowHeight="15660" xr2:uid="{42C517F9-3C2F-4E44-A03E-BA06A54FC42C}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
     <sheet name="Cadastro" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:J9"/>
+  <oleSize ref="A1:I19"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -22,14 +22,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
   <si>
     <t>Usuario</t>
   </si>
   <si>
-    <t>Roger</t>
-  </si>
-  <si>
     <t>Senha</t>
   </si>
   <si>
@@ -108,16 +105,16 @@
     <t>09030601</t>
   </si>
   <si>
-    <t>VictorAlbanoV17</t>
-  </si>
-  <si>
-    <t>victoralbanoV17@gmail.com</t>
-  </si>
-  <si>
     <t>Victor</t>
   </si>
   <si>
     <t>11953459764</t>
+  </si>
+  <si>
+    <t>AlbanoVictor17</t>
+  </si>
+  <si>
+    <t>AlbanoVictor17@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -537,8 +534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82DFF3C8-B17A-4903-B3D2-C0FC0EFDC6B7}">
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -558,24 +555,24 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H1" s="7"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25"/>
@@ -591,8 +588,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{502FE14B-E947-42A8-81A3-4901D77307AB}">
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -612,104 +609,104 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>14</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="G2" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="I2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="J2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="5" t="s">
-        <v>20</v>
-      </c>
       <c r="K2" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="6" t="s">
+      <c r="D3" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="E3" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="F3" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="5" t="s">
-        <v>25</v>
-      </c>
       <c r="G3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="I3" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="J3" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="5" t="s">
-        <v>20</v>
-      </c>
       <c r="K3" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>